<commit_message>
Updated various design documents
</commit_message>
<xml_diff>
--- a/Design Documents/Narration/Narrative Data/Infos.xlsx
+++ b/Design Documents/Narration/Narrative Data/Infos.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremias/Desktop/UNIL/MASTER/PROJET_ISH/ijo-musi/Design Documents/Narration/Narrative Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C94F78-2119-5449-9F27-7BA3FDF8CE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8660BC01-D8BB-FB44-856F-F0F6161FB32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="27340" windowHeight="17260" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="27340" windowHeight="17260" activeTab="1" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
   </bookViews>
   <sheets>
     <sheet name="Narration" sheetId="1" r:id="rId1"/>
-    <sheet name="toki pona" sheetId="2" r:id="rId2"/>
+    <sheet name="proto scenes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="323">
   <si>
     <t>Name</t>
   </si>
@@ -431,9 +431,6 @@
     <t>∗ The Loose One fled the temple after the Shaped One confronted them on their manipulation. (Mid-Late)</t>
   </si>
   <si>
-    <t>∗ Using the tool on the Enlightened One’s grave, the Shaped One heard a confession of the Rigid One, begging pardon to the Enlightened One for his actions (but the nature pof the actions remain a mystery). (Mid-Late)</t>
-  </si>
-  <si>
     <t>∗ The Shaped One had a suspicion that the Enlightened One's death was no accident. (Mid-Late)</t>
   </si>
   <si>
@@ -443,9 +440,6 @@
     <t xml:space="preserve">∗ The secondary reason for the fight: the Rigid One is responsible for the death of the Enlightened One. (Late) </t>
   </si>
   <si>
-    <t>∗ The Shaped One confronted the Rigid One for the murders of the Enlightened One. (Late)</t>
-  </si>
-  <si>
     <t>suicide</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
   </si>
   <si>
     <t>Ideas and notes</t>
-  </si>
-  <si>
-    <t>EO says that what is is, and what is is sacred. "ale li sewi", echoing the sentence said by LO in the plant scene.</t>
   </si>
   <si>
     <t>…</t>
@@ -514,11 +505,6 @@
     <t>Lock Prayer Room behind puzzle?</t>
   </si>
   <si>
-    <t>&lt;&gt; Identifying the flask as the same type as another one clearly labelled poison
-&lt;&gt; Fighting scene (linked to broken main door)
-&lt;&gt; Suicide letter</t>
-  </si>
-  <si>
     <t>&lt;&gt; Flask
 &lt;&gt; Suicide letter</t>
   </si>
@@ -671,10 +657,6 @@
 &lt;&gt; RO's Room</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;&gt; EO's pendant
-&lt;&gt; </t>
-  </si>
-  <si>
     <t>&lt;&gt; Murals (Waiting Room)
 &lt;&gt; Prayer scene (linked to lectern)</t>
   </si>
@@ -698,38 +680,398 @@
 &lt;&gt; West Staircase</t>
   </si>
   <si>
+    <t>&lt;&gt; West Staircase</t>
+  </si>
+  <si>
+    <t>&lt;&gt; RO's mural explanation to LO scene (linked to Prayer Room mural)</t>
+  </si>
+  <si>
+    <t>RO secret room access</t>
+  </si>
+  <si>
+    <t>∗ RO accessed the secret room to take the mirror and to put it back.</t>
+  </si>
+  <si>
+    <t>EO's hope</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Secret Room</t>
+  </si>
+  <si>
+    <t>&lt;&gt; EO's message to SO.</t>
+  </si>
+  <si>
+    <t>&lt;&gt; RO's Secret Room explanation to SO scene (linked to Secret Room door)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; RO's eloge of EO to SO scene. (linked to EO's tomb)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Kitchen</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Crops</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Wasing Station</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Washing Station</t>
+  </si>
+  <si>
+    <t>&lt;&gt; West Staircase
+&lt;&gt; East Staircase</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Washing Station
+&lt;&gt; Crops
+&lt;&gt; Kitchen
+&lt;&gt; Library</t>
+  </si>
+  <si>
+    <t>∗ Using the tool on the Enlightened One’s grave, the Shaped One heard a confession of the Rigid One, begging pardon to the Enlightened One for his actions (but the nature of the actions remain a mystery). (Mid-Late)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Hall</t>
+  </si>
+  <si>
+    <t>∗ The Shaped One confronted the Rigid One for the murder of the Enlightened One. (Late)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Balcony</t>
+  </si>
+  <si>
+    <t>&lt;&gt; LO's Room</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Dining Room
+&lt;&gt; RO's Room</t>
+  </si>
+  <si>
+    <t>&lt;&gt; East Staircase</t>
+  </si>
+  <si>
+    <t>∗ EO hoped for the artificial people to become a freer and better version of humans.</t>
+  </si>
+  <si>
+    <t>&lt;&gt; …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; … </t>
+  </si>
+  <si>
+    <t>broken barrier</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>* The barrier on the Balcony is broken (Mid)</t>
+  </si>
+  <si>
     <t>&lt;&gt; The Secret Room is visible from the Balcony.
-&lt;&gt; The door to the Secret Room arise in the West Staircase.</t>
-  </si>
-  <si>
-    <t>&lt;&gt; West Staircase</t>
-  </si>
-  <si>
-    <t>&lt;&gt; RO's mural explanation to LO scene (linked to Prayer Room mural)</t>
-  </si>
-  <si>
-    <t>RO secret room access</t>
-  </si>
-  <si>
-    <t>∗ RO accessed the secret room to take the mirror and to put it back.</t>
-  </si>
-  <si>
-    <t>EO's hope</t>
-  </si>
-  <si>
-    <t>∗ EO hoped for the artificial people to become afreer and better version of humans.</t>
-  </si>
-  <si>
-    <t>&lt;&gt; Secret Room</t>
-  </si>
-  <si>
-    <t>&lt;&gt; EO's message to SO.</t>
-  </si>
-  <si>
-    <t>&lt;&gt; RO's Secret Room explanation to SO scene (linked to Secret Room door)</t>
-  </si>
-  <si>
-    <t>&lt;&gt; RO's eloge of EO to SO scene. (linked to EO's tomb)</t>
+&lt;&gt; The door to the Secret Room stands in the West Staircase.</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Fight scene 1/3 (linked to empty poison bottle)</t>
+  </si>
+  <si>
+    <t>The fight starts there, then goes to the hall, then to the library, which is burnt at this point(?)
+The empty bottle rests on the cliff, behind the broken barrier.</t>
+  </si>
+  <si>
+    <t>Maybe no scene, just the murals ?</t>
+  </si>
+  <si>
+    <t>Literraly only sound of scratching and RO swearing "pakala!"</t>
+  </si>
+  <si>
+    <t>&lt;&gt; "pakala !" scene (linked to piece of frame stuck in the scratch on the wall)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Player has to make the link between piece of frame and rest of frame in the Pond</t>
+  </si>
+  <si>
+    <t>The frame should have a unique color. Texture won't be seen with ascii filter. Maybe wood with golden decoration? Why not sitelen sitelen decoration even?</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Forbidding scene (linked to the "keep out" sign on the barricade)</t>
+  </si>
+  <si>
+    <t>The sign and "barricade" are broken (SO broke them when they went to visit the grave)
+We can hear RO nail the sign to the barricade in the scene.</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Confession scene (linked to grave)
+&lt;&gt; Fight scene 1/3 (linked to poison bottle on Balcony)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Sacred Resting Place
+&lt;&gt; Balcony</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Waiting</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Plants scene (linked to plants)</t>
+  </si>
+  <si>
+    <t>EO says that what is is, and what is is sacred. "ale li sewi", echoing the sentence said by LO in the plant scene.
+EO asks to be left alone with RO.
+Something like "I do wish you used a less painful way to make me go."
+Maybe atlk about the fact that they mistook their own enlightenment for the ability to teach it.</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Death scene (linked to tree)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Sacred Resting Place
+&lt;&gt; Craft Room ?
+&lt;&gt; Prayer Room</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Mirror frame (Pond)
+&lt;&gt; Murals (Prayer Room)</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Argument scene (linked to discarded clay head)</t>
+  </si>
+  <si>
+    <t>"You need to work on your own awareness before you bring a new one into the world"</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Waiting Room
+&lt;&gt; Crops</t>
+  </si>
+  <si>
+    <t>&lt;&gt; RO blames LO scene (linked to broken plant pot)</t>
+  </si>
+  <si>
+    <t>Add breaking of pot in this scene ?</t>
+  </si>
+  <si>
+    <t>Have RO be sweet/gentle towards SO. Make the lin between the broken clay pot and the fear that LO will break the clay person (SO).</t>
+  </si>
+  <si>
+    <t>&lt;&gt; EO's pendant
+&lt;&gt; Make link between global info and suicide letter</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Balcony
+&lt;&gt; Hall
+&lt;&gt; Library
+&lt;&gt; Waiting Room</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Fight scenes 1-3
+&lt;&gt; Suicide Letter</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Instruction on walls.</t>
+  </si>
+  <si>
+    <t>There is no doors to the secret room, just walls with the inscriptions. And the scratch that stops mid-wall is a clue that the wall opens.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>sentence</t>
+  </si>
+  <si>
+    <t>infos</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>hidden_words</t>
+  </si>
+  <si>
+    <t>dialog</t>
+  </si>
+  <si>
+    <t>fight_1</t>
+  </si>
+  <si>
+    <t>argument</t>
+  </si>
+  <si>
+    <t>ro_mural_explanation_to_lo</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>pakala</t>
+  </si>
+  <si>
+    <t>forbidding</t>
+  </si>
+  <si>
+    <t>confession</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>awakening</t>
+  </si>
+  <si>
+    <t>ro_eloge_of_eo_to_so</t>
+  </si>
+  <si>
+    <t>ro_blames_lo</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>"The Shaped One confronted the Rigid One for the murder of the Enlightened One. (Late)",
+"The Rigid One commited suicide after the Shaped One left, and after some harsh but true words. (Mid-Late)"</t>
+  </si>
+  <si>
+    <t>&lt;&gt; Identifying the flask as the same type as another one clearly labelled poison
+&lt;&gt; Fighting scene 2/3 (linked to broken main door)
+&lt;&gt; Suicide letter</t>
+  </si>
+  <si>
+    <t>balcony</t>
+  </si>
+  <si>
+    <t>poison_bottle</t>
+  </si>
+  <si>
+    <t>craft_room</t>
+  </si>
+  <si>
+    <t>clay_head</t>
+  </si>
+  <si>
+    <t>craft_room_mural</t>
+  </si>
+  <si>
+    <t>waiting_room</t>
+  </si>
+  <si>
+    <t>dead_plants</t>
+  </si>
+  <si>
+    <t>east_staircase</t>
+  </si>
+  <si>
+    <t>frame_in_wall</t>
+  </si>
+  <si>
+    <t>pond</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>resting_place</t>
+  </si>
+  <si>
+    <t>grave</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>mirror_frame</t>
+  </si>
+  <si>
+    <t>drawings_on_wall</t>
+  </si>
+  <si>
+    <t>broken_pot</t>
+  </si>
+  <si>
+    <t>dice</t>
+  </si>
+  <si>
+    <t>"The Rigid One was pushing for the creation of the Shaped One, but the
+Enlightened One considered them not to be ready. (Mid)"</t>
+  </si>
+  <si>
+    <t>"The artificial person was supposed to become a ”perfect mind”. (Mid)",
+"The cult wanted to use toki pona to shape the mind of the clay-person. (Mid)"</t>
+  </si>
+  <si>
+    <t>"RO accessed the secret room to take the mirror and to put it back."</t>
+  </si>
+  <si>
+    <t>"The Rigid One forbid the Shaped One to use the tool on the Enlightened
+One’s grave. (Mid)"</t>
+  </si>
+  <si>
+    <t>"Using the tool on the Enlightened One’s grave, the Shaped One heard a confession of the Rigid One, begging pardon to the Enlightened One for his actions (but the nature of the actions remain a mystery). (Mid-Late)"</t>
+  </si>
+  <si>
+    <t>"The Enlightened One knew the meal was poisonned. (Late)"</t>
+  </si>
+  <si>
+    <t>"The Enlightened One was using the tool as a key for the secret room. (Mid)"</t>
+  </si>
+  <si>
+    <t>"The cult succeeded in creating the clay-person. (Early-Mid)",
+"The Shaped One knew nothing at first. (Early-Mid)"</t>
+  </si>
+  <si>
+    <t>"The Shaped One realized that the Loose One was manipulative after a
+talk with the Rigid One. (Mid-Late)"</t>
+  </si>
+  <si>
+    <t>"The Loose One and the Shaped One had fun together. (Early-Mid)"</t>
+  </si>
+  <si>
+    <t>"The Loose One tended to neglect her duties. (Early)",
+"The Rigid One tended to give orders to the others. (Early)",
+"The barrier on the Balcony is broken (Mid)"</t>
+  </si>
+  <si>
+    <t>"kasi ni li moli."</t>
+  </si>
+  <si>
+    <t>ro_last_moments</t>
+  </si>
+  <si>
+    <t>ro_skeleton</t>
+  </si>
+  <si>
+    <t>"jan ni li moli. sijelo kiwen ona li awen anpa."</t>
+  </si>
+  <si>
+    <t>moli</t>
+  </si>
+  <si>
+    <t>poki, pakala</t>
+  </si>
+  <si>
+    <t>"lawa pi ko kiwen."</t>
+  </si>
+  <si>
+    <t>"poki ni li pakala."</t>
+  </si>
+  <si>
+    <t>lawa, kiwen</t>
+  </si>
+  <si>
+    <t>clues</t>
+  </si>
+  <si>
+    <t>"sitelen suli ni li pana lukin e jan pali pi ko kiwen"</t>
+  </si>
+  <si>
+    <t>sitelen, lukin, ko</t>
+  </si>
+  <si>
+    <t>&lt;&gt; "kasi xxx", "kasi yyy", etc physical labels on the plants. Only in sitelen pona
+&lt;&gt; skeleton sentence contains "moli"
+&lt;&gt; dead fish in pond that can be revived (yellow object)</t>
   </si>
 </sst>
 </file>
@@ -783,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -797,11 +1139,119 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1045,24 +1495,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}" name="Table1" displayName="Table1" ref="A1:J73" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J73" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J73">
-    <sortCondition ref="F1:F73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}" name="Table1" displayName="Table1" ref="A1:J74" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:J74" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J74">
+    <sortCondition ref="D1:D74"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A3972590-6843-E64D-BC8B-BE7F61021465}" name="Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C3FDF78C-9C8A-384C-A991-91CE1FE2E698}" name="Mystery" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B29A1B80-6D4C-4B4E-8DDE-8665F64956DF}" name="Info" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8A8BB49C-F3B9-124C-AAA9-B71B4638E352}" name="Room" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{FB141D1B-4AA2-5546-ABCB-9120591D12F1}" name="Medium" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D8B5D0BC-C917-6243-9E21-EFCAC6482479}" name="Timing / 5" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{0B157806-E1A4-6043-AA30-D1E15F12C568}" name="Findable" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{51D56085-B0C3-E841-B846-C22EDBD243D9}" name="Understandable" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{29BFBE76-ABF1-5E49-B5EE-417D1C8C1B44}" name="Difficulty" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{A3972590-6843-E64D-BC8B-BE7F61021465}" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C3FDF78C-9C8A-384C-A991-91CE1FE2E698}" name="Mystery" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{B29A1B80-6D4C-4B4E-8DDE-8665F64956DF}" name="Info" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8A8BB49C-F3B9-124C-AAA9-B71B4638E352}" name="Room" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{FB141D1B-4AA2-5546-ABCB-9120591D12F1}" name="Medium" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{D8B5D0BC-C917-6243-9E21-EFCAC6482479}" name="Timing / 5" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{0B157806-E1A4-6043-AA30-D1E15F12C568}" name="Findable" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{51D56085-B0C3-E841-B846-C22EDBD243D9}" name="Understandable" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{29BFBE76-ABF1-5E49-B5EE-417D1C8C1B44}" name="Difficulty" dataDxfId="17">
       <calculatedColumnFormula xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{44F0299F-D12F-334D-95A5-FD753E4B8195}" name="Ideas and notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{44F0299F-D12F-334D-95A5-FD753E4B8195}" name="Ideas and notes" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8B0A543-28F6-294F-8B07-E17D8AA06C2B}" name="Table3" displayName="Table3" ref="A1:H14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+  <autoFilter ref="A1:H14" xr:uid="{A8B0A543-28F6-294F-8B07-E17D8AA06C2B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1355E863-F6E3-D349-91CC-66026BF92E65}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{11B5C82D-9182-164A-AC1A-C7860136E82F}" name="infos" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A4DAD171-1D30-194C-B63A-3BC9D929AA6C}" name="place" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{FD04A320-3781-4743-BBB2-47BBED4853F8}" name="object" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{6A83D1B3-B3D1-824B-A40A-3434A2205F56}" name="sentence" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A3C2C38B-7967-F649-A4A6-C189FCD5B493}" name="hidden_words" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{5217A8AB-14D0-7B41-B779-58D056DC5244}" name="clues" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{929F8BC9-DAB2-A945-B46C-9F9644C93C91}" name="dialog" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1365,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E12883-83E3-F048-A22A-B025C2FD18CF}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="B1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1406,16 +1873,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
@@ -1429,10 +1896,10 @@
         <v>121</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1448,783 +1915,666 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="I4" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>199</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>2.2360679774997898</v>
+        <v>4.1231056256176606</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.1622776601683795</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.1622776601683795</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>3.1622776601683795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="2">
-        <v>3</v>
-      </c>
-      <c r="I8" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>3</v>
-      </c>
       <c r="I9" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>148</v>
+        <v>204</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2">
         <v>4</v>
       </c>
       <c r="H10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.6568542494923806</v>
+        <v>4.4721359549995796</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
         <v>1</v>
       </c>
-      <c r="H11" s="2">
-        <v>2</v>
-      </c>
       <c r="I11" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>2.2360679774997898</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2</v>
-      </c>
-      <c r="H12" s="2">
         <v>3</v>
       </c>
       <c r="I12" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
+        <v>213</v>
       </c>
       <c r="I13" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.1231056256176606</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
         <v>3</v>
       </c>
-      <c r="H14" s="2">
-        <v>3</v>
-      </c>
       <c r="I14" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.2426406871192848</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>
       </c>
       <c r="G15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>3.6055512754639891</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
       <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="I16" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
         <v>2</v>
-      </c>
-      <c r="G16" s="2">
-        <v>4</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>4</v>
       </c>
       <c r="H17" s="2">
         <v>3</v>
       </c>
       <c r="I17" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>163</v>
+        <v>3.6055512754639891</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>168</v>
+        <v>243</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
       <c r="H18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
+        <v>3.6055512754639891</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F20" s="2">
-        <v>2</v>
-      </c>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="I20" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>6</v>
+        <v>206</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>164</v>
+        <v>224</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="2">
-        <v>2</v>
-      </c>
-      <c r="G21" s="2">
-        <v>3</v>
-      </c>
-      <c r="H21" s="2">
-        <v>5</v>
+        <v>236</v>
       </c>
       <c r="I21" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>224</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="F22" s="2">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I22" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
         <v>3</v>
       </c>
       <c r="I23" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2">
-        <v>2</v>
-      </c>
-      <c r="H24" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I24" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>6.324555320336759</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="F25" s="2">
-        <v>2</v>
-      </c>
-      <c r="G25" s="2">
+        <v>3</v>
+      </c>
+      <c r="I25" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
         <v>4</v>
       </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
-      <c r="I25" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>6.4031242374328485</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="H26" s="2">
         <v>4</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F26" s="4">
-        <v>3</v>
-      </c>
-      <c r="I26" s="4">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="I26" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="F27" s="2">
         <v>3</v>
       </c>
-      <c r="G27" s="2">
-        <v>4</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2</v>
-      </c>
       <c r="I27" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>4</v>
@@ -2239,106 +2589,88 @@
     </row>
     <row r="29" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="2">
         <v>5</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F29" s="2">
-        <v>3</v>
-      </c>
-      <c r="G29" s="2">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
       <c r="I29" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.0990195135927845</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
         <v>5</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F30" s="2">
-        <v>3</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>4</v>
-      </c>
-      <c r="I30" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.1231056256176606</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F31" s="2">
-        <v>3</v>
+      <c r="H31" s="2">
+        <v>2</v>
       </c>
       <c r="I31" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>206</v>
+        <v>49</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>218</v>
+        <v>164</v>
       </c>
       <c r="F32" s="2">
         <v>3</v>
@@ -2348,21 +2680,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>217</v>
+        <v>164</v>
       </c>
       <c r="F33" s="2">
         <v>3</v>
@@ -2372,15 +2701,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="F34" s="2">
         <v>3</v>
@@ -2390,87 +2722,126 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="F35" s="2">
+        <v>2</v>
+      </c>
+      <c r="G35" s="2">
+        <v>5</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>5.3851648071345037</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I36" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2">
+        <v>5</v>
+      </c>
+      <c r="H37" s="2">
         <v>3</v>
       </c>
-      <c r="I35" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" s="2">
-        <v>3</v>
-      </c>
-      <c r="I36" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="2">
-        <v>3</v>
-      </c>
       <c r="I37" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>40</v>
+        <v>186</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="F38" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1</v>
       </c>
       <c r="I38" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>41</v>
+        <v>95</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F39" s="2">
         <v>3</v>
@@ -2480,69 +2851,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F40" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I40" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F41" s="2">
+        <v>5</v>
+      </c>
+      <c r="I41" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="2">
+        <v>2</v>
+      </c>
+      <c r="G42" s="2">
+        <v>4</v>
+      </c>
+      <c r="H42" s="2">
         <v>3</v>
       </c>
-      <c r="I41" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="2">
-        <v>3</v>
-      </c>
       <c r="I42" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="F43" s="2">
         <v>3</v>
@@ -2551,70 +2949,106 @@
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J43" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>49</v>
+        <v>218</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="F44" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I44" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F45" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I45" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+      <c r="J45" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F46" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G46" s="2">
+        <v>4</v>
+      </c>
+      <c r="H46" s="2">
+        <v>5</v>
       </c>
       <c r="I46" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+        <v>6.4031242374328485</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>52</v>
+        <v>201</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="F47" s="2">
         <v>3</v>
@@ -2624,36 +3058,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="F48" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2</v>
       </c>
       <c r="I48" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>22</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="F49" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I49" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2662,85 +3114,112 @@
     </row>
     <row r="50" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F50" s="2">
+        <v>2</v>
+      </c>
+      <c r="G50" s="2">
+        <v>4</v>
+      </c>
+      <c r="H50" s="2">
+        <v>2</v>
+      </c>
+      <c r="I50" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>4.4721359549995796</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" s="2">
+        <v>6</v>
+      </c>
+      <c r="I51" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="C52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" s="2">
         <v>3</v>
       </c>
-      <c r="I50" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F51" s="2">
-        <v>4</v>
-      </c>
-      <c r="I51" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="I52" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F53" s="2">
         <v>5</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" s="2">
-        <v>4</v>
-      </c>
-      <c r="I52" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F53" s="2">
-        <v>4</v>
-      </c>
       <c r="I53" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="F54" s="2">
         <v>4</v>
@@ -2750,15 +3229,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>31</v>
+        <v>129</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="F55" s="2">
         <v>4</v>
@@ -2770,49 +3252,82 @@
     </row>
     <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F56" s="2">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G56" s="2">
+        <v>5</v>
+      </c>
+      <c r="H56" s="2">
+        <v>1</v>
       </c>
       <c r="I56" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="F57" s="2">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G57" s="2">
+        <v>3</v>
+      </c>
+      <c r="H57" s="2">
+        <v>3</v>
       </c>
       <c r="I57" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>129</v>
+        <v>42</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="F58" s="2">
         <v>4</v>
@@ -2821,273 +3336,446 @@
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J58" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="F59" s="2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1</v>
       </c>
       <c r="I59" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>131</v>
+        <v>15</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="F60" s="2">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G60" s="2">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
       </c>
       <c r="I60" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F61" s="2">
+        <v>2</v>
+      </c>
+      <c r="G61" s="2">
+        <v>2</v>
+      </c>
+      <c r="H61" s="2">
+        <v>6</v>
+      </c>
+      <c r="I61" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>6.324555320336759</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F62" s="2">
+        <v>4</v>
+      </c>
+      <c r="I62" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F63" s="2">
+        <v>2</v>
+      </c>
+      <c r="G63" s="2">
+        <v>3</v>
+      </c>
+      <c r="H63" s="2">
         <v>5</v>
       </c>
-      <c r="I61" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="I63" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F64" s="2">
+        <v>2</v>
+      </c>
+      <c r="G64" s="2">
+        <v>5</v>
+      </c>
+      <c r="H64" s="2">
+        <v>3</v>
+      </c>
+      <c r="I64" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F65" s="2">
+        <v>3</v>
+      </c>
+      <c r="I65" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F62" s="2">
-        <v>5</v>
-      </c>
-      <c r="I62" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F63" s="2">
-        <v>5</v>
-      </c>
-      <c r="I63" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F64" s="2">
-        <v>5</v>
-      </c>
-      <c r="I64" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F65" s="2">
-        <v>5</v>
-      </c>
-      <c r="I65" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C66" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="F66" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I66" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>128</v>
+        <v>175</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="I67" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>144</v>
+        <v>38</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F68" s="2">
+        <v>4</v>
       </c>
       <c r="I68" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>167</v>
+        <v>37</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F69" s="2">
+        <v>2</v>
+      </c>
+      <c r="G69" s="2">
+        <v>5</v>
+      </c>
+      <c r="H69" s="2">
+        <v>2</v>
       </c>
       <c r="I69" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+        <v>5.3851648071345037</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>180</v>
+        <v>45</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" s="2">
+        <v>3</v>
       </c>
       <c r="I70" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" s="2">
+        <v>3</v>
       </c>
       <c r="I71" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>213</v>
+        <v>81</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>214</v>
+        <v>25</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F72" s="2">
+        <v>3</v>
       </c>
       <c r="I72" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>188</v>
+        <v>80</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>189</v>
+        <v>24</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="F73" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I73" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I74" s="5">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="East">
+      <formula>NOT(ISERROR(SEARCH("East",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Waiting">
+      <formula>NOT(ISERROR(SEARCH("Waiting",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Sacred">
+      <formula>NOT(ISERROR(SEARCH("Sacred",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Pond">
+      <formula>NOT(ISERROR(SEARCH("Pond",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Balcony">
+      <formula>NOT(ISERROR(SEARCH("Balcony",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Craft">
+      <formula>NOT(ISERROR(SEARCH("Craft",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3097,12 +3785,260 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDF2BC-5ADE-0B4A-AAFC-D255F3A83AC7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="40.83203125" style="7"/>
+    <col min="3" max="3" width="16.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="40.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wrote some scenes and worked on click feature of ilo toki
</commit_message>
<xml_diff>
--- a/Design Documents/Narration/Narrative Data/Infos.xlsx
+++ b/Design Documents/Narration/Narrative Data/Infos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremias/Desktop/UNIL/MASTER/PROJET_ISH/ijo-musi/Design Documents/Narration/Narrative Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8660BC01-D8BB-FB44-856F-F0F6161FB32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2B35A-C75D-3D45-8D42-240790AAB786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="27340" windowHeight="17260" activeTab="1" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28520" windowHeight="17260" activeTab="1" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
   </bookViews>
   <sheets>
     <sheet name="Narration" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="336">
   <si>
     <t>Name</t>
   </si>
@@ -1072,6 +1072,45 @@
     <t>&lt;&gt; "kasi xxx", "kasi yyy", etc physical labels on the plants. Only in sitelen pona
 &lt;&gt; skeleton sentence contains "moli"
 &lt;&gt; dead fish in pond that can be revived (yellow object)</t>
+  </si>
+  <si>
+    <t>Scenes I would like to add</t>
+  </si>
+  <si>
+    <t>Choosing a name</t>
+  </si>
+  <si>
+    <t>SO and LO call RO by an insulting name</t>
+  </si>
+  <si>
+    <t>Ro changes their name</t>
+  </si>
+  <si>
+    <t>RO: "ko jaki!", RO: "pakala a!"</t>
+  </si>
+  <si>
+    <t>"lipu ni li pakala."</t>
+  </si>
+  <si>
+    <t>lipu, pakala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*sounds of hammering nails*, SO: "jan RO! sina pali e seme?", RO: "a! jan SO! sina lon la, ni li pona tawa mi.",  SO: "sina pini e lupa tawa tomo moli pi mama sewi anu seme?", RO: "mi pini e ni. tenpo kama la, sina ken ala tawa tomo moli.", SO: "tan seme?", RO: "tan mi toki e ni.", *small silence*, SO: "tan seme?", RO: "tan tomo moli ni li sewi. mama sewi li moli. jan moli li wile e lape." SO: "taso-" *So gets cut off* RO: "taso ala a! mi toki e ijo la, ijo ni li lon! o weka!" </t>
+  </si>
+  <si>
+    <t>RO: "sitelen suli ni li pana lukin e ko wawa", LO: "ko ni li wawa tan seme?", "RO: ko ni li sewi. ni li ken kama ale.", LO: "ale?!", RO: "poka.", LO: "ni li ken kama jan?", RO: "mi pilin e ni, taso tenpo pini la, ni li kama ala.",</t>
+  </si>
+  <si>
+    <t>RO: "mi lon… tenpo pini suli la, mi lon ala. taso, tenpo ni la, mi lon… mi pilin ike... lawa ona mute li utala. sina sona e ni. tenpo sina moli ala la, sina toki e ni... tenpo pini la, mi pakala e sina. taso, tenpo ni la, mi wile e ni ala... mi pakala. mi pakala suli."</t>
+  </si>
+  <si>
+    <t>"tomo moli li toki e ni: ''jan XXX. sina lawa e mi mute. sina sona e sewi. sina toki pona. moli sina li pilin ike tawa mi mute.''"</t>
+  </si>
+  <si>
+    <t>moli, toki, e, ike, mute, XXX</t>
+  </si>
+  <si>
+    <t>SO: "jan XXX!", RO: "jan XXX. toki.", SO: "o toki e lon!", RO: "sina toki e seme?", *sound of searching through something, then sound of liquid in bottle*, "ni! sina sona e poki ni anu seme?!", *silence*, RO: "sina tawa insa e tomo mi? sina ken ala e ni. sina sona e ni.", SO: "tenpo ni la, ni li suli ala.", *RO cutting SO off*, RO: "ni li suli a! mi lawa. mi toki e ijo la, sina kute e ni!", SO: "pakala a! o pakala e sina! sina moli e jan XXX! sina moli e mama sewi!", RO: "o kalama ala! toki sina li ike. ni li lon ala. sina sona e ala! o pana mi e pakala poki ni!", SO: "ala a! o sina tawa mi ala!", *struggling sounds*, RO: "o pana!", SO: "ala!" *more struggling sounds, sound of bottle hitting ground then rolling*,  SO: "pakala! poki li tawa anpa...", RO: "o kute-", *RO gets cut off*, "ala! tenpo pini la, mi kepeken ilo toki e tomo moli pi mama sewi. ni la, mi kute e sina toki tawa ona. mi kute sina toki e lon. sina moli e jan XXX!", *silence*, RO: "mi-" *gets cut off*, SO: "mi tawa." *sounds of steps leaving*, RO: "ala! o awen!"</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1109,6 +1148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1125,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1137,9 +1182,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,13 +1199,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1224,33 +1302,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1495,10 +1546,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}" name="Table1" displayName="Table1" ref="A1:J74" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:J74" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J74">
-    <sortCondition ref="D1:D74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}" name="Table1" displayName="Table1" ref="A1:J78" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:J78" xr:uid="{A333011E-814B-4044-8CEE-912E2F961A31}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J78">
+    <sortCondition ref="B1:B78"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A3972590-6843-E64D-BC8B-BE7F61021465}" name="Name" dataDxfId="25"/>
@@ -1519,17 +1570,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8B0A543-28F6-294F-8B07-E17D8AA06C2B}" name="Table3" displayName="Table3" ref="A1:H14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8B0A543-28F6-294F-8B07-E17D8AA06C2B}" name="Table3" displayName="Table3" ref="A1:H14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H14" xr:uid="{A8B0A543-28F6-294F-8B07-E17D8AA06C2B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
+    <sortCondition ref="C1:C14"/>
+  </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1355E863-F6E3-D349-91CC-66026BF92E65}" name="id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{11B5C82D-9182-164A-AC1A-C7860136E82F}" name="infos" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A4DAD171-1D30-194C-B63A-3BC9D929AA6C}" name="place" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{FD04A320-3781-4743-BBB2-47BBED4853F8}" name="object" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{6A83D1B3-B3D1-824B-A40A-3434A2205F56}" name="sentence" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{A3C2C38B-7967-F649-A4A6-C189FCD5B493}" name="hidden_words" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{5217A8AB-14D0-7B41-B779-58D056DC5244}" name="clues" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{929F8BC9-DAB2-A945-B46C-9F9644C93C91}" name="dialog" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{1355E863-F6E3-D349-91CC-66026BF92E65}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{11B5C82D-9182-164A-AC1A-C7860136E82F}" name="infos" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A4DAD171-1D30-194C-B63A-3BC9D929AA6C}" name="place" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FD04A320-3781-4743-BBB2-47BBED4853F8}" name="object" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{6A83D1B3-B3D1-824B-A40A-3434A2205F56}" name="sentence" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A3C2C38B-7967-F649-A4A6-C189FCD5B493}" name="hidden_words" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{5217A8AB-14D0-7B41-B779-58D056DC5244}" name="clues" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{929F8BC9-DAB2-A945-B46C-9F9644C93C91}" name="dialog" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1832,9 +1886,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E12883-83E3-F048-A22A-B025C2FD18CF}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1885,48 +1939,48 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
       <c r="I2" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>227</v>
+        <v>154</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="F3" s="2">
         <v>3</v>
@@ -1935,265 +1989,214 @@
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>220</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F4" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4</v>
+        <v>213</v>
       </c>
       <c r="I5" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.1231056256176606</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>2.2360679774997898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>249</v>
+        <v>177</v>
       </c>
       <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
         <v>3</v>
       </c>
       <c r="I7" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>250</v>
+        <v>3.6055512754639891</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="F8" s="2">
+        <v>3</v>
+      </c>
+      <c r="I8" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
         <v>3</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>3.6055512754639891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="I8" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.1622776601683795</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
         <v>3</v>
       </c>
-      <c r="G9" s="2">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2</v>
-      </c>
-      <c r="I9" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F10" s="2">
-        <v>3</v>
-      </c>
-      <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2</v>
-      </c>
       <c r="I10" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>234</v>
+        <v>3.6055512754639891</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
         <v>3</v>
       </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
       <c r="I11" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.1622776601683795</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="I12" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2202,34 +2205,40 @@
     </row>
     <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>213</v>
+        <v>224</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="I13" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="F14" s="2">
         <v>3</v>
@@ -2241,148 +2250,145 @@
     </row>
     <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2">
         <v>3</v>
       </c>
       <c r="I15" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="F16" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2">
+        <v>4</v>
       </c>
       <c r="I16" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>2</v>
-      </c>
-      <c r="H17" s="2">
         <v>3</v>
       </c>
       <c r="I17" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>2</v>
-      </c>
-      <c r="H18" s="2">
-        <v>3</v>
+        <v>222</v>
       </c>
       <c r="I18" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>3.6055512754639891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>143</v>
+        <v>178</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="F19" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
       </c>
       <c r="I19" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>223</v>
+        <v>164</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
       </c>
       <c r="I20" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2391,112 +2397,112 @@
     </row>
     <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>205</v>
+        <v>109</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>236</v>
+        <v>164</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3</v>
       </c>
       <c r="I21" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>237</v>
+        <v>164</v>
       </c>
       <c r="F22" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I22" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>219</v>
+        <v>157</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="F23" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
       </c>
       <c r="I23" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>4.1231056256176606</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="F24" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="F25" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I25" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2505,49 +2511,44 @@
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>145</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <v>4</v>
-      </c>
-      <c r="H26" s="2">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.6568542494923806</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>144</v>
+        <v>171</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="F27" s="2">
         <v>3</v>
@@ -2556,49 +2557,49 @@
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>144</v>
+        <v>242</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>161</v>
+        <v>241</v>
       </c>
       <c r="F28" s="2">
-        <v>2</v>
-      </c>
-      <c r="G28" s="2">
         <v>4</v>
       </c>
-      <c r="H28" s="2">
-        <v>2</v>
-      </c>
       <c r="I28" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>131</v>
+        <v>32</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>144</v>
+        <v>171</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F29" s="2">
         <v>5</v>
@@ -2607,73 +2608,88 @@
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J29" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>222</v>
+        <v>139</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2</v>
       </c>
       <c r="I30" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>2.2360679774997898</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H31" s="2">
         <v>2</v>
       </c>
       <c r="I31" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>183</v>
+        <v>4.4721359549995796</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>49</v>
+        <v>185</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>164</v>
+        <v>208</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="F32" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2682,19 +2698,19 @@
     </row>
     <row r="33" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F33" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I33" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2703,19 +2719,19 @@
     </row>
     <row r="34" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F34" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I34" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2724,169 +2740,169 @@
     </row>
     <row r="35" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F35" s="2">
         <v>2</v>
       </c>
       <c r="G35" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H35" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
+        <v>4.2426406871192848</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>207</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>225</v>
+        <v>42</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>164</v>
+        <v>251</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F36" s="2">
+        <v>4</v>
       </c>
       <c r="I36" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J36" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="F37" s="2">
-        <v>2</v>
-      </c>
-      <c r="G37" s="2">
-        <v>5</v>
-      </c>
-      <c r="H37" s="2">
         <v>3</v>
       </c>
       <c r="I37" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F38" s="2">
-        <v>2</v>
-      </c>
-      <c r="G38" s="2">
-        <v>4</v>
-      </c>
-      <c r="H38" s="2">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="I38" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.1231056256176606</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="F39" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I39" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>157</v>
+        <v>182</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="F40" s="2">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2">
         <v>5</v>
       </c>
+      <c r="H40" s="2">
+        <v>2</v>
+      </c>
       <c r="I40" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>5.3851648071345037</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="F41" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I41" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -2895,271 +2911,292 @@
     </row>
     <row r="42" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>157</v>
+      <c r="C42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="F42" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F43" s="2">
         <v>3</v>
       </c>
+      <c r="G43" s="2">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
+        <v>4</v>
+      </c>
       <c r="I43" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+        <v>4.1231056256176606</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>218</v>
+        <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>242</v>
+        <v>154</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>241</v>
+        <v>155</v>
       </c>
       <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+      <c r="I44" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>3.1622776601683795</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F45" s="2">
+        <v>3</v>
+      </c>
+      <c r="G45" s="2">
         <v>4</v>
       </c>
-      <c r="I44" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F45" s="2">
-        <v>5</v>
+      <c r="H45" s="2">
+        <v>2</v>
       </c>
       <c r="I45" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>4.4721359549995796</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="F46" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G46" s="2">
         <v>4</v>
       </c>
       <c r="H46" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I46" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>6.4031242374328485</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
       <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2">
         <v>3</v>
       </c>
+      <c r="H47" s="2">
+        <v>1</v>
+      </c>
       <c r="I47" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>139</v>
+        <v>224</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>138</v>
+        <v>237</v>
       </c>
       <c r="F48" s="2">
-        <v>1</v>
-      </c>
-      <c r="G48" s="2">
-        <v>1</v>
-      </c>
-      <c r="H48" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I48" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>2.2360679774997898</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>247</v>
+        <v>144</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
       <c r="F49" s="2">
+        <v>2</v>
+      </c>
+      <c r="G49" s="2">
         <v>4</v>
       </c>
+      <c r="H49" s="2">
+        <v>2</v>
+      </c>
       <c r="I49" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+        <v>4.4721359549995796</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="F50" s="2">
         <v>2</v>
       </c>
       <c r="G50" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H50" s="2">
         <v>2</v>
       </c>
       <c r="I50" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.4721359549995796</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>5.3851648071345037</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F51" s="2">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="I51" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3168,187 +3205,217 @@
     </row>
     <row r="52" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>208</v>
+        <v>166</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="F52" s="2">
+        <v>2</v>
+      </c>
+      <c r="G52" s="2">
+        <v>5</v>
+      </c>
+      <c r="H52" s="2">
         <v>3</v>
       </c>
       <c r="I52" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>208</v>
+        <v>157</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="F53" s="2">
+        <v>2</v>
+      </c>
+      <c r="G53" s="2">
+        <v>4</v>
+      </c>
+      <c r="H53" s="2">
+        <v>3</v>
+      </c>
+      <c r="I53" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>5</v>
       </c>
-      <c r="I53" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
+      <c r="J53" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F54" s="2">
+        <v>2</v>
+      </c>
+      <c r="G54" s="2">
         <v>4</v>
       </c>
+      <c r="H54" s="2">
+        <v>5</v>
+      </c>
       <c r="I54" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>6.4031242374328485</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>129</v>
+        <v>201</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="F55" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I55" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>170</v>
+        <v>247</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>173</v>
+        <v>248</v>
       </c>
       <c r="F56" s="2">
-        <v>3</v>
-      </c>
-      <c r="G56" s="2">
-        <v>5</v>
-      </c>
-      <c r="H56" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I56" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.0990195135927845</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F57" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G57" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H57" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>4.2426406871192848</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>251</v>
+        <v>152</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>252</v>
+        <v>153</v>
       </c>
       <c r="F58" s="2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
       </c>
       <c r="I58" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>254</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>152</v>
@@ -3370,84 +3437,81 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="F60" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G60" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H60" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I60" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="F61" s="2">
-        <v>2</v>
-      </c>
-      <c r="G61" s="2">
-        <v>2</v>
-      </c>
-      <c r="H61" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I61" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>6.324555320336759</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>256</v>
+        <v>203</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="F62" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I62" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3456,103 +3520,94 @@
     </row>
     <row r="63" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F63" s="2">
         <v>4</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F63" s="2">
-        <v>2</v>
-      </c>
-      <c r="G63" s="2">
-        <v>3</v>
-      </c>
-      <c r="H63" s="2">
-        <v>5</v>
-      </c>
       <c r="I63" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
+        <v>0</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="F64" s="2">
-        <v>2</v>
-      </c>
-      <c r="G64" s="2">
-        <v>5</v>
-      </c>
-      <c r="H64" s="2">
         <v>3</v>
       </c>
       <c r="I64" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.8309518948453007</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>255</v>
+        <v>191</v>
       </c>
       <c r="F65" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G65" s="2">
+        <v>1</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2</v>
       </c>
       <c r="I65" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F66" s="2">
         <v>3</v>
@@ -3562,172 +3617,175 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>176</v>
+        <v>208</v>
+      </c>
+      <c r="F67" s="2">
+        <v>5</v>
       </c>
       <c r="I67" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F68" s="2">
+        <v>5</v>
+      </c>
+      <c r="I68" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I68" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C69" s="2" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="F69" s="2">
-        <v>2</v>
-      </c>
-      <c r="G69" s="2">
         <v>5</v>
       </c>
-      <c r="H69" s="2">
-        <v>2</v>
-      </c>
       <c r="I69" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>5.3851648071345037</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>214</v>
+        <v>156</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F70" s="2">
+        <v>2</v>
+      </c>
+      <c r="G70" s="2">
+        <v>2</v>
+      </c>
+      <c r="H70" s="2">
+        <v>6</v>
+      </c>
+      <c r="I70" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>6.324555320336759</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F71" s="2">
+        <v>4</v>
+      </c>
+      <c r="I71" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F72" s="2">
+        <v>2</v>
+      </c>
+      <c r="G72" s="2">
         <v>3</v>
       </c>
-      <c r="I70" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B71" s="2" t="s">
+      <c r="H72" s="2">
         <v>5</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F71" s="2">
+      <c r="I72" s="2">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F73" s="2">
         <v>3</v>
       </c>
-      <c r="I71" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F72" s="2">
-        <v>3</v>
-      </c>
-      <c r="I72" s="2">
-        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F73" s="2">
-        <v>4</v>
-      </c>
       <c r="I73" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="18" x14ac:dyDescent="0.2">
@@ -3746,33 +3804,69 @@
       <c r="E74" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I74" s="5">
+      <c r="I74" s="2">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
         <v>0</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="I75" s="12">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I76" s="10">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I77" s="10">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I78" s="10">
+        <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="East">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="East">
       <formula>NOT(ISERROR(SEARCH("East",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Waiting">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Waiting">
       <formula>NOT(ISERROR(SEARCH("Waiting",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Sacred">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Sacred">
       <formula>NOT(ISERROR(SEARCH("Sacred",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Pond">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Pond">
       <formula>NOT(ISERROR(SEARCH("Pond",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Balcony">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Balcony">
       <formula>NOT(ISERROR(SEARCH("Balcony",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Craft">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Craft">
       <formula>NOT(ISERROR(SEARCH("Craft",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3787,251 +3881,286 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDF2BC-5ADE-0B4A-AAFC-D255F3A83AC7}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="40.83203125" style="7"/>
-    <col min="3" max="3" width="16.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="40.83203125" style="7"/>
+    <col min="1" max="2" width="40.83203125" style="6"/>
+    <col min="3" max="3" width="16.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="40.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>315</v>
       </c>
+      <c r="H2" s="6" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="H4" s="6" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
     <row r="12" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>298</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wrote some prototype scenes
</commit_message>
<xml_diff>
--- a/Design Documents/Narration/Narrative Data/Infos.xlsx
+++ b/Design Documents/Narration/Narrative Data/Infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremias/Desktop/UNIL/MASTER/PROJET_ISH/ijo-musi/Design Documents/Narration/Narrative Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2B35A-C75D-3D45-8D42-240790AAB786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58A723-CE7F-FC40-B79F-21178391636E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28520" windowHeight="17260" activeTab="1" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="337">
   <si>
     <t>Name</t>
   </si>
@@ -1051,13 +1051,7 @@
     <t>poki, pakala</t>
   </si>
   <si>
-    <t>"lawa pi ko kiwen."</t>
-  </si>
-  <si>
     <t>"poki ni li pakala."</t>
-  </si>
-  <si>
-    <t>lawa, kiwen</t>
   </si>
   <si>
     <t>clues</t>
@@ -1111,6 +1105,15 @@
   </si>
   <si>
     <t>SO: "jan XXX!", RO: "jan XXX. toki.", SO: "o toki e lon!", RO: "sina toki e seme?", *sound of searching through something, then sound of liquid in bottle*, "ni! sina sona e poki ni anu seme?!", *silence*, RO: "sina tawa insa e tomo mi? sina ken ala e ni. sina sona e ni.", SO: "tenpo ni la, ni li suli ala.", *RO cutting SO off*, RO: "ni li suli a! mi lawa. mi toki e ijo la, sina kute e ni!", SO: "pakala a! o pakala e sina! sina moli e jan XXX! sina moli e mama sewi!", RO: "o kalama ala! toki sina li ike. ni li lon ala. sina sona e ala! o pana mi e pakala poki ni!", SO: "ala a! o sina tawa mi ala!", *struggling sounds*, RO: "o pana!", SO: "ala!" *more struggling sounds, sound of bottle hitting ground then rolling*,  SO: "pakala! poki li tawa anpa...", RO: "o kute-", *RO gets cut off*, "ala! tenpo pini la, mi kepeken ilo toki e tomo moli pi mama sewi. ni la, mi kute e sina toki tawa ona. mi kute sina toki e lon. sina moli e jan XXX!", *silence*, RO: "mi-" *gets cut off*, SO: "mi tawa." *sounds of steps leaving*, RO: "ala! o awen!"</t>
+  </si>
+  <si>
+    <t>"lawa pi ko."</t>
+  </si>
+  <si>
+    <t>lawa, ko</t>
+  </si>
+  <si>
+    <t>EO: "jan XXX! sina pali e seme?", RO: "ni li lawa pi ko wawa.", EO: "mi lukin e ni. taso sina pali e ni tan seme?", RO: "tan tenpo kama la, jan pona tan ko li wile e lawa.", EO: "taso tenpo ni la, jan pi ko li lon ala.", RO: "taso tenpo kama lili, ni li lon.", EO: "jan XXX... sina sona e nasin sewi sina li pini ala.", RO: "sina toki e ni: ''tenpo ala la, nasin sewi li pini'', EO: "ni li lon. pona a! sina kama sona mute! ni li pona tawa mi.", *silence*, EO: "taso, tenpo pi jan pona tan ko li tenpo ni ala.", *grunt*, RO: "tan seme? mi kute e toki sewi tan sina. sona mi li suli a!", *tssk tssk sound*, EO: "ala. sona sina li lili.", RO: "taso-", *cut off*, EO: "sona jan XX li lili, sona sina li lili. sona mi li lili. ale la, sona mi mute li lili.", RO: "ala a! jan XXX li sona lili. sina li sona mute. mi li sona.", EO: "sina toki ike. toki ni li pona ala.", *silence*, EO: "o kama. tenpo moku li lon."</t>
   </si>
 </sst>
 </file>
@@ -3814,7 +3817,7 @@
     </row>
     <row r="75" spans="1:10" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I75" s="12">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3823,7 +3826,7 @@
     </row>
     <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I76" s="10">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3832,7 +3835,7 @@
     </row>
     <row r="77" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I77" s="10">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3841,7 +3844,7 @@
     </row>
     <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I78" s="10">
         <f xml:space="preserve"> SQRT((Table1[[#This Row],[Understandable]]^2) + (Table1[[#This Row],[Findable]]^2))</f>
@@ -3914,7 +3917,7 @@
         <v>265</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>266</v>
@@ -3934,13 +3937,13 @@
         <v>282</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>315</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -3957,10 +3960,13 @@
         <v>284</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>318</v>
+        <v>335</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -3977,13 +3983,13 @@
         <v>285</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -4000,7 +4006,7 @@
         <v>289</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -4017,13 +4023,13 @@
         <v>291</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,13 +4078,13 @@
         <v>293</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="9" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
@@ -4119,7 +4125,7 @@
         <v>314</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added link between red mode of tool and label resources
</commit_message>
<xml_diff>
--- a/Design Documents/Narration/Narrative Data/Infos.xlsx
+++ b/Design Documents/Narration/Narrative Data/Infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremias/Desktop/UNIL/MASTER/PROJET_ISH/ijo-musi/Design Documents/Narration/Narrative Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58A723-CE7F-FC40-B79F-21178391636E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79C74D7-87EF-7B48-9562-23B94A960A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="28520" windowHeight="17260" activeTab="1" xr2:uid="{09E5F364-D8F4-704D-9AEF-8348B3D4D38B}"/>
   </bookViews>
@@ -3884,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDF2BC-5ADE-0B4A-AAFC-D255F3A83AC7}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40.83203125" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>